<commit_message>
including data (also in idynomics protocol units)
</commit_message>
<xml_diff>
--- a/protocol/calibration test/dataset_nitrification.xlsx
+++ b/protocol/calibration test/dataset_nitrification.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="11565"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="11565" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="original" sheetId="1" r:id="rId1"/>
+    <sheet name="idyno" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,21 +16,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>oxygen</t>
+    <t>time (days)</t>
   </si>
   <si>
-    <t>ammonium</t>
+    <t>oxygen (mgO2/l)</t>
   </si>
   <si>
-    <t>nitrite</t>
+    <t>ammonium (mgN/l)</t>
   </si>
   <si>
-    <t>nitrate</t>
+    <t>nitrite (mgN/l)</t>
   </si>
   <si>
-    <t>time (days)</t>
+    <t>nitrate (mgN/l)</t>
+  </si>
+  <si>
+    <t>time (min)</t>
+  </si>
+  <si>
+    <t>oxygen (pgO2/fl)</t>
+  </si>
+  <si>
+    <t>ammonium (pgN/fl)</t>
+  </si>
+  <si>
+    <t>nitrite (pgN/fl)</t>
+  </si>
+  <si>
+    <t>nitrate (pgN/fl)</t>
   </si>
 </sst>
 </file>
@@ -371,31 +386,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1000,12 +1018,809 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>original!A2*24*60</f>
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <f>original!B2*0.000001</f>
+        <v>8.0081879165104996E-6</v>
+      </c>
+      <c r="C2">
+        <f>original!C2*0.000001</f>
+        <v>2.0004303958479399E-5</v>
+      </c>
+      <c r="D2">
+        <f>original!D2*0.000001</f>
+        <v>8.3751201275772402E-8</v>
+      </c>
+      <c r="E2">
+        <f>original!E2*0.000001</f>
+        <v>3.6462600274069301E-8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>original!A3*24*60</f>
+        <v>4.9999999999999964</v>
+      </c>
+      <c r="B3">
+        <f>original!B3*0.000001</f>
+        <v>3.8294136291512601E-6</v>
+      </c>
+      <c r="C3">
+        <f>original!C3*0.000001</f>
+        <v>1.7739219320434099E-5</v>
+      </c>
+      <c r="D3">
+        <f>original!D3*0.000001</f>
+        <v>2.1890790822883297E-6</v>
+      </c>
+      <c r="E3">
+        <f>original!E3*0.000001</f>
+        <v>-7.2737451965667895E-9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>original!A4*24*60</f>
+        <v>9.9999999999999929</v>
+      </c>
+      <c r="B4">
+        <f>original!B4*0.000001</f>
+        <v>2.8852600658083596E-6</v>
+      </c>
+      <c r="C4">
+        <f>original!C4*0.000001</f>
+        <v>1.5607430889522499E-5</v>
+      </c>
+      <c r="D4">
+        <f>original!D4*0.000001</f>
+        <v>4.3008419895635498E-6</v>
+      </c>
+      <c r="E4">
+        <f>original!E4*0.000001</f>
+        <v>-4.6332330959104901E-9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f>original!A5*24*60</f>
+        <v>15.00000000000005</v>
+      </c>
+      <c r="B5">
+        <f>original!B5*0.000001</f>
+        <v>2.7196443148277496E-6</v>
+      </c>
+      <c r="C5">
+        <f>original!C5*0.000001</f>
+        <v>1.37241379836396E-5</v>
+      </c>
+      <c r="D5">
+        <f>original!D5*0.000001</f>
+        <v>6.4526526982711194E-6</v>
+      </c>
+      <c r="E5">
+        <f>original!E5*0.000001</f>
+        <v>3.6731085112802597E-8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f>original!A6*24*60</f>
+        <v>20.000000000000014</v>
+      </c>
+      <c r="B6">
+        <f>original!B6*0.000001</f>
+        <v>2.7045667225685299E-6</v>
+      </c>
+      <c r="C6">
+        <f>original!C6*0.000001</f>
+        <v>1.16304081683078E-5</v>
+      </c>
+      <c r="D6">
+        <f>original!D6*0.000001</f>
+        <v>8.39766594866601E-6</v>
+      </c>
+      <c r="E6">
+        <f>original!E6*0.000001</f>
+        <v>-3.4159664754420199E-8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f>original!A7*24*60</f>
+        <v>24.999999999999986</v>
+      </c>
+      <c r="B7">
+        <f>original!B7*0.000001</f>
+        <v>2.7029188151127796E-6</v>
+      </c>
+      <c r="C7">
+        <f>original!C7*0.000001</f>
+        <v>9.6500321993419891E-6</v>
+      </c>
+      <c r="D7">
+        <f>original!D7*0.000001</f>
+        <v>1.0341448081777099E-5</v>
+      </c>
+      <c r="E7">
+        <f>original!E7*0.000001</f>
+        <v>4.5112619416349896E-8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f>original!A8*24*60</f>
+        <v>29.999999999999954</v>
+      </c>
+      <c r="B8">
+        <f>original!B8*0.000001</f>
+        <v>2.72735358666902E-6</v>
+      </c>
+      <c r="C8">
+        <f>original!C8*0.000001</f>
+        <v>7.6970806222334996E-6</v>
+      </c>
+      <c r="D8">
+        <f>original!D8*0.000001</f>
+        <v>1.24007656141287E-5</v>
+      </c>
+      <c r="E8">
+        <f>original!E8*0.000001</f>
+        <v>3.4300825813231301E-8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>original!A9*24*60</f>
+        <v>35.000000000000064</v>
+      </c>
+      <c r="B9">
+        <f>original!B9*0.000001</f>
+        <v>2.7993208486200098E-6</v>
+      </c>
+      <c r="C9">
+        <f>original!C9*0.000001</f>
+        <v>5.6285999737139298E-6</v>
+      </c>
+      <c r="D9">
+        <f>original!D9*0.000001</f>
+        <v>1.4284130946422299E-5</v>
+      </c>
+      <c r="E9">
+        <f>original!E9*0.000001</f>
+        <v>-1.2145748168882401E-8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f>original!A10*24*60</f>
+        <v>40.000000000000028</v>
+      </c>
+      <c r="B10">
+        <f>original!B10*0.000001</f>
+        <v>2.8852999049354998E-6</v>
+      </c>
+      <c r="C10">
+        <f>original!C10*0.000001</f>
+        <v>3.66094233565302E-6</v>
+      </c>
+      <c r="D10">
+        <f>original!D10*0.000001</f>
+        <v>1.6219790146440998E-5</v>
+      </c>
+      <c r="E10">
+        <f>original!E10*0.000001</f>
+        <v>8.9727250358840704E-8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f>original!A11*24*60</f>
+        <v>45</v>
+      </c>
+      <c r="B11">
+        <f>original!B11*0.000001</f>
+        <v>3.1206048561293496E-6</v>
+      </c>
+      <c r="C11">
+        <f>original!C11*0.000001</f>
+        <v>1.8651287515804699E-6</v>
+      </c>
+      <c r="D11">
+        <f>original!D11*0.000001</f>
+        <v>1.81603697545651E-5</v>
+      </c>
+      <c r="E11">
+        <f>original!E11*0.000001</f>
+        <v>-9.1756620650756187E-8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f>original!A12*24*60</f>
+        <v>49.999999999999972</v>
+      </c>
+      <c r="B12">
+        <f>original!B12*0.000001</f>
+        <v>3.9628855264484896E-6</v>
+      </c>
+      <c r="C12">
+        <f>original!C12*0.000001</f>
+        <v>3.1759588336041599E-7</v>
+      </c>
+      <c r="D12">
+        <f>original!D12*0.000001</f>
+        <v>1.9507049582700299E-5</v>
+      </c>
+      <c r="E12">
+        <f>original!E12*0.000001</f>
+        <v>7.3094252400433787E-8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f>original!A13*24*60</f>
+        <v>54.999999999999936</v>
+      </c>
+      <c r="B13">
+        <f>original!B13*0.000001</f>
+        <v>6.2875165796135496E-6</v>
+      </c>
+      <c r="C13">
+        <f>original!C13*0.000001</f>
+        <v>-4.0898701812742203E-8</v>
+      </c>
+      <c r="D13">
+        <f>original!D13*0.000001</f>
+        <v>1.9973214529644297E-5</v>
+      </c>
+      <c r="E13">
+        <f>original!E13*0.000001</f>
+        <v>-1.4234365769112599E-9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f>original!A14*24*60</f>
+        <v>60.000000000000057</v>
+      </c>
+      <c r="B14">
+        <f>original!B14*0.000001</f>
+        <v>7.4660450947143102E-6</v>
+      </c>
+      <c r="C14">
+        <f>original!C14*0.000001</f>
+        <v>7.7718999987865091E-9</v>
+      </c>
+      <c r="D14">
+        <f>original!D14*0.000001</f>
+        <v>2.0059962247140799E-5</v>
+      </c>
+      <c r="E14">
+        <f>original!E14*0.000001</f>
+        <v>-6.3447535007330495E-8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f>original!A15*24*60</f>
+        <v>65.000000000000028</v>
+      </c>
+      <c r="B15">
+        <f>original!B15*0.000001</f>
+        <v>7.8440839547427903E-6</v>
+      </c>
+      <c r="C15">
+        <f>original!C15*0.000001</f>
+        <v>-8.9574183621358982E-9</v>
+      </c>
+      <c r="D15">
+        <f>original!D15*0.000001</f>
+        <v>1.99538617182214E-5</v>
+      </c>
+      <c r="E15">
+        <f>original!E15*0.000001</f>
+        <v>1.5276689414393398E-8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f>original!A16*24*60</f>
+        <v>69.999999999999972</v>
+      </c>
+      <c r="B16">
+        <f>original!B16*0.000001</f>
+        <v>7.9442346724154388E-6</v>
+      </c>
+      <c r="C16">
+        <f>original!C16*0.000001</f>
+        <v>8.4819334720657505E-8</v>
+      </c>
+      <c r="D16">
+        <f>original!D16*0.000001</f>
+        <v>2.0115660524223401E-5</v>
+      </c>
+      <c r="E16">
+        <f>original!E16*0.000001</f>
+        <v>-5.9024792978332895E-8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f>original!A17*24*60</f>
+        <v>74.999999999999943</v>
+      </c>
+      <c r="B17">
+        <f>original!B17*0.000001</f>
+        <v>7.9687019785528201E-6</v>
+      </c>
+      <c r="C17">
+        <f>original!C17*0.000001</f>
+        <v>3.8564879983487896E-8</v>
+      </c>
+      <c r="D17">
+        <f>original!D17*0.000001</f>
+        <v>2.00581091252431E-5</v>
+      </c>
+      <c r="E17">
+        <f>original!E17*0.000001</f>
+        <v>1.1987248361165899E-7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f>original!A18*24*60</f>
+        <v>80.000000000000057</v>
+      </c>
+      <c r="B18">
+        <f>original!B18*0.000001</f>
+        <v>7.9907204527592198E-6</v>
+      </c>
+      <c r="C18">
+        <f>original!C18*0.000001</f>
+        <v>8.3642847846274797E-9</v>
+      </c>
+      <c r="D18">
+        <f>original!D18*0.000001</f>
+        <v>1.9918775759723496E-5</v>
+      </c>
+      <c r="E18">
+        <f>original!E18*0.000001</f>
+        <v>3.13451442792357E-8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f>original!A19*24*60</f>
+        <v>85.000000000000028</v>
+      </c>
+      <c r="B19">
+        <f>original!B19*0.000001</f>
+        <v>7.9695664034203402E-6</v>
+      </c>
+      <c r="C19">
+        <f>original!C19*0.000001</f>
+        <v>2.1813706550798597E-8</v>
+      </c>
+      <c r="D19">
+        <f>original!D19*0.000001</f>
+        <v>2.00492566809314E-5</v>
+      </c>
+      <c r="E19">
+        <f>original!E19*0.000001</f>
+        <v>-9.4952198341338693E-8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f>original!A20*24*60</f>
+        <v>90</v>
+      </c>
+      <c r="B20">
+        <f>original!B20*0.000001</f>
+        <v>7.9963579371179294E-6</v>
+      </c>
+      <c r="C20">
+        <f>original!C20*0.000001</f>
+        <v>1.58600392580984E-8</v>
+      </c>
+      <c r="D20">
+        <f>original!D20*0.000001</f>
+        <v>1.9926004418391599E-5</v>
+      </c>
+      <c r="E20">
+        <f>original!E20*0.000001</f>
+        <v>-3.7604654804669793E-8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f>original!A21*24*60</f>
+        <v>94.999999999999957</v>
+      </c>
+      <c r="B21">
+        <f>original!B21*0.000001</f>
+        <v>7.9781363147221093E-6</v>
+      </c>
+      <c r="C21">
+        <f>original!C21*0.000001</f>
+        <v>1.3060223655588499E-8</v>
+      </c>
+      <c r="D21">
+        <f>original!D21*0.000001</f>
+        <v>1.9943366100353401E-5</v>
+      </c>
+      <c r="E21">
+        <f>original!E21*0.000001</f>
+        <v>-4.3564715690266196E-10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f>original!A22*24*60</f>
+        <v>100.00000000000009</v>
+      </c>
+      <c r="B22">
+        <f>original!B22*0.000001</f>
+        <v>7.97332998876254E-6</v>
+      </c>
+      <c r="C22">
+        <f>original!C22*0.000001</f>
+        <v>-1.8569612229986598E-9</v>
+      </c>
+      <c r="D22">
+        <f>original!D22*0.000001</f>
+        <v>2.0096024677669598E-5</v>
+      </c>
+      <c r="E22">
+        <f>original!E22*0.000001</f>
+        <v>-2.3418094819348101E-8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f>original!A23*24*60</f>
+        <v>105.00000000000006</v>
+      </c>
+      <c r="B23">
+        <f>original!B23*0.000001</f>
+        <v>7.9948516286632401E-6</v>
+      </c>
+      <c r="C23">
+        <f>original!C23*0.000001</f>
+        <v>-4.4935780761416202E-8</v>
+      </c>
+      <c r="D23">
+        <f>original!D23*0.000001</f>
+        <v>2.0050647874003099E-5</v>
+      </c>
+      <c r="E23">
+        <f>original!E23*0.000001</f>
+        <v>2.5631215561466799E-8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f>original!A24*24*60</f>
+        <v>110.00000000000001</v>
+      </c>
+      <c r="B24">
+        <f>original!B24*0.000001</f>
+        <v>7.9597277481888304E-6</v>
+      </c>
+      <c r="C24">
+        <f>original!C24*0.000001</f>
+        <v>3.8832456298488799E-8</v>
+      </c>
+      <c r="D24">
+        <f>original!D24*0.000001</f>
+        <v>2.0101541539315198E-5</v>
+      </c>
+      <c r="E24">
+        <f>original!E24*0.000001</f>
+        <v>-9.7274791031238296E-8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f>original!A25*24*60</f>
+        <v>114.99999999999999</v>
+      </c>
+      <c r="B25">
+        <f>original!B25*0.000001</f>
+        <v>7.9668887880196303E-6</v>
+      </c>
+      <c r="C25">
+        <f>original!C25*0.000001</f>
+        <v>1.2173140961646099E-8</v>
+      </c>
+      <c r="D25">
+        <f>original!D25*0.000001</f>
+        <v>2.0062667036948499E-5</v>
+      </c>
+      <c r="E25">
+        <f>original!E25*0.000001</f>
+        <v>5.1131859041315397E-8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f>original!A26*24*60</f>
+        <v>119.99999999999994</v>
+      </c>
+      <c r="B26">
+        <f>original!B26*0.000001</f>
+        <v>7.9778070644993E-6</v>
+      </c>
+      <c r="C26">
+        <f>original!C26*0.000001</f>
+        <v>-5.6389489465415994E-8</v>
+      </c>
+      <c r="D26">
+        <f>original!D26*0.000001</f>
+        <v>2.0013614862393696E-5</v>
+      </c>
+      <c r="E26">
+        <f>original!E26*0.000001</f>
+        <v>-8.0330852054359304E-8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f>original!A27*24*60</f>
+        <v>125.00000000000006</v>
+      </c>
+      <c r="B27">
+        <f>original!B27*0.000001</f>
+        <v>7.9916937062382101E-6</v>
+      </c>
+      <c r="C27">
+        <f>original!C27*0.000001</f>
+        <v>-3.6051201838833699E-8</v>
+      </c>
+      <c r="D27">
+        <f>original!D27*0.000001</f>
+        <v>2.0076977385939302E-5</v>
+      </c>
+      <c r="E27">
+        <f>original!E27*0.000001</f>
+        <v>-5.5026676623694694E-8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f>original!A28*24*60</f>
+        <v>130.00000000000006</v>
+      </c>
+      <c r="B28">
+        <f>original!B28*0.000001</f>
+        <v>7.9839294601286893E-6</v>
+      </c>
+      <c r="C28">
+        <f>original!C28*0.000001</f>
+        <v>-1.4586199334341799E-8</v>
+      </c>
+      <c r="D28">
+        <f>original!D28*0.000001</f>
+        <v>1.9914934798444099E-5</v>
+      </c>
+      <c r="E28">
+        <f>original!E28*0.000001</f>
+        <v>-3.7893623392886694E-8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f>original!A29*24*60</f>
+        <v>135</v>
+      </c>
+      <c r="B29">
+        <f>original!B29*0.000001</f>
+        <v>7.9832006622519204E-6</v>
+      </c>
+      <c r="C29">
+        <f>original!C29*0.000001</f>
+        <v>-4.5757295491921798E-8</v>
+      </c>
+      <c r="D29">
+        <f>original!D29*0.000001</f>
+        <v>2.0025836438252098E-5</v>
+      </c>
+      <c r="E29">
+        <f>original!E29*0.000001</f>
+        <v>1.2734406084136602E-7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f>original!A30*24*60</f>
+        <v>139.99999999999994</v>
+      </c>
+      <c r="B30">
+        <f>original!B30*0.000001</f>
+        <v>7.9742361069198296E-6</v>
+      </c>
+      <c r="C30">
+        <f>original!C30*0.000001</f>
+        <v>1.0516272322074999E-8</v>
+      </c>
+      <c r="D30">
+        <f>original!D30*0.000001</f>
+        <v>1.99782401967428E-5</v>
+      </c>
+      <c r="E30">
+        <f>original!E30*0.000001</f>
+        <v>-2.1818843729296398E-8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f>original!A31*24*60</f>
+        <v>144.99999999999937</v>
+      </c>
+      <c r="B31">
+        <f>original!B31*0.000001</f>
+        <v>7.9468525932375194E-6</v>
+      </c>
+      <c r="C31">
+        <f>original!C31*0.000001</f>
+        <v>4.4554697851307999E-9</v>
+      </c>
+      <c r="D31">
+        <f>original!D31*0.000001</f>
+        <v>2.0002968507135299E-5</v>
+      </c>
+      <c r="E31">
+        <f>original!E31*0.000001</f>
+        <v>6.7266577540342689E-8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f>original!A32*24*60</f>
+        <v>150.00000000000048</v>
+      </c>
+      <c r="B32">
+        <f>original!B32*0.000001</f>
+        <v>7.9623898251200492E-6</v>
+      </c>
+      <c r="C32">
+        <f>original!C32*0.000001</f>
+        <v>-5.1839191558586197E-8</v>
+      </c>
+      <c r="D32">
+        <f>original!D32*0.000001</f>
+        <v>2.0055973975160299E-5</v>
+      </c>
+      <c r="E32">
+        <f>original!E32*0.000001</f>
+        <v>-5.0625764523192793E-8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f>original!A33*24*60</f>
+        <v>155.00000000000017</v>
+      </c>
+      <c r="B33">
+        <f>original!B33*0.000001</f>
+        <v>7.97929892817841E-6</v>
+      </c>
+      <c r="C33">
+        <f>original!C33*0.000001</f>
+        <v>9.2172078440061507E-8</v>
+      </c>
+      <c r="D33">
+        <f>original!D33*0.000001</f>
+        <v>2.0080172043215101E-5</v>
+      </c>
+      <c r="E33">
+        <f>original!E33*0.000001</f>
+        <v>-5.0984036093485992E-9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f>original!A34*24*60</f>
+        <v>159.99999999999983</v>
+      </c>
+      <c r="B34">
+        <f>original!B34*0.000001</f>
+        <v>7.9785815312304296E-6</v>
+      </c>
+      <c r="C34">
+        <f>original!C34*0.000001</f>
+        <v>-1.0009484996679199E-7</v>
+      </c>
+      <c r="D34">
+        <f>original!D34*0.000001</f>
+        <v>1.9975450045909899E-5</v>
+      </c>
+      <c r="E34">
+        <f>original!E34*0.000001</f>
+        <v>7.8688020276818893E-8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f>original!A35*24*60</f>
+        <v>164.99999999999952</v>
+      </c>
+      <c r="B35">
+        <f>original!B35*0.000001</f>
+        <v>7.9899547359841807E-6</v>
+      </c>
+      <c r="C35">
+        <f>original!C35*0.000001</f>
+        <v>-2.3306822038915699E-8</v>
+      </c>
+      <c r="D35">
+        <f>original!D35*0.000001</f>
+        <v>1.9952685552285101E-5</v>
+      </c>
+      <c r="E35">
+        <f>original!E35*0.000001</f>
+        <v>-2.6424449368708101E-8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f>original!A36*24*60</f>
+        <v>170.00000000000063</v>
+      </c>
+      <c r="B36">
+        <f>original!B36*0.000001</f>
+        <v>7.9838611713833389E-6</v>
+      </c>
+      <c r="C36">
+        <f>original!C36*0.000001</f>
+        <v>4.1714161255785197E-8</v>
+      </c>
+      <c r="D36">
+        <f>original!D36*0.000001</f>
+        <v>1.9989325920539998E-5</v>
+      </c>
+      <c r="E36">
+        <f>original!E36*0.000001</f>
+        <v>3.9392684486451702E-8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>